<commit_message>
resolved data type bugs
</commit_message>
<xml_diff>
--- a/kiba_labs_data_sheet_new.xlsx
+++ b/kiba_labs_data_sheet_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28627"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28706"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nabeel\AIDIPH-LIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC14A2AD-7C0D-4ED3-A3F0-261709245A57}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D4CBEA-6389-40A4-9301-35B7527CCDEE}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="5" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="17" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organisation_details" sheetId="1" r:id="rId1"/>
@@ -3330,7 +3330,7 @@
     <t>prorata_basis</t>
   </si>
   <si>
-    <t>causal</t>
+    <t>casual</t>
   </si>
   <si>
     <t>HOLIDAY MANAGEMENT</t>
@@ -3501,10 +3501,10 @@
     <t>Morning shift</t>
   </si>
   <si>
-    <t>2025-02-25T09:00:00</t>
-  </si>
-  <si>
-    <t>2025-02-25T18:00:00</t>
+    <t>2024-01-01T9:00:00</t>
+  </si>
+  <si>
+    <t>2024-01-01T5:30:00</t>
   </si>
   <si>
     <t>Standard morning shift with 1 hour break</t>
@@ -3516,10 +3516,10 @@
     <t>flexible</t>
   </si>
   <si>
-    <t>2025-02-27T09:00:00</t>
-  </si>
-  <si>
-    <t>2025-02-27T18:00:00</t>
+    <t>2024-01-01T6:30:00</t>
+  </si>
+  <si>
+    <t>2024-01-01T1:30:00</t>
   </si>
   <si>
     <t>Flexible timing with 2 hours window</t>
@@ -3535,7 +3535,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3629,6 +3629,12 @@
       <color rgb="FFFF0000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -3745,7 +3751,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3765,6 +3771,7 @@
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -4109,20 +4116,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:31" ht="14.45" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:31" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -4355,20 +4362,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>299</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
     </row>
     <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -4525,16 +4532,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -4630,17 +4637,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -4766,7 +4773,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46F7946E-EEA5-43D3-BE03-CE5CA6F9110C}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
@@ -4790,23 +4797,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>333</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -4908,7 +4915,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB38F180-2F2C-4017-A0FF-9CF8FF5EDE00}">
   <dimension ref="A1:R26"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScale="120" workbookViewId="0">
+    <sheetView zoomScale="120" workbookViewId="0">
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
@@ -4935,26 +4942,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -5077,7 +5084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCFD0342-AB7E-4371-A9B1-8F7F40D3C79F}">
   <dimension ref="A1:V3"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" zoomScale="116" workbookViewId="0">
+    <sheetView zoomScale="116" workbookViewId="0">
       <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
@@ -5105,30 +5112,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
-      <c r="U1" s="15"/>
-      <c r="V1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
+      <c r="U1" s="16"/>
+      <c r="V1" s="16"/>
     </row>
     <row r="2" spans="1:22" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -5278,7 +5285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C55244-73ED-4C00-9AAA-1CE3088AB3F0}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
+    <sheetView topLeftCell="E8" workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -5302,22 +5309,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -5436,17 +5443,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="1" t="s">
@@ -5516,8 +5523,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{771473C8-0ED1-48AE-9391-29EDA379D213}">
   <dimension ref="A1:X6"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q20" sqref="Q20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -5549,26 +5556,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="14.45" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>348</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
     </row>
     <row r="2" spans="1:24" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -5749,17 +5756,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>408</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -5960,30 +5967,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="14.45" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="19"/>
     </row>
     <row r="2" spans="1:22" ht="15.6">
       <c r="A2" s="13" t="s">
@@ -6188,8 +6195,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{586F6509-5C69-49DF-BED7-4ABA7FC1FBF4}">
   <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AD2" sqref="AD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6230,27 +6237,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="14.45" customHeight="1">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
     </row>
     <row r="2" spans="1:34" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -6459,7 +6466,7 @@
   <dimension ref="A1:S4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6468,7 +6475,8 @@
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="23" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="21.85546875" bestFit="1" customWidth="1"/>
@@ -6482,27 +6490,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
     </row>
     <row r="2" spans="1:19" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -6554,7 +6562,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="3" spans="1:19">
+    <row r="3" spans="1:19" ht="15">
       <c r="A3" t="s">
         <v>463</v>
       </c>
@@ -6567,10 +6575,10 @@
       <c r="D3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="15" t="s">
         <v>464</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="15" t="s">
         <v>465</v>
       </c>
       <c r="H3">
@@ -6601,7 +6609,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="4" spans="1:19">
+    <row r="4" spans="1:19" ht="15">
       <c r="A4" t="s">
         <v>467</v>
       </c>
@@ -6614,10 +6622,10 @@
       <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="15" t="s">
         <v>469</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" s="15" t="s">
         <v>470</v>
       </c>
       <c r="G4">
@@ -6683,17 +6691,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>427</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -6827,7 +6835,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6845,19 +6853,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="19"/>
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="14" t="s">
@@ -6971,8 +6979,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BD60CA-9150-40C0-B868-C9DA9FAE1363}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -7012,32 +7020,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:34" ht="21" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
+      <c r="W1" s="18"/>
+      <c r="X1" s="19"/>
     </row>
     <row r="2" spans="1:34" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -7333,7 +7341,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.45">
+    <row r="5" spans="1:34">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -7452,8 +7460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACE41A9A-53B4-4989-87EB-2AE81B794EBA}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7475,22 +7483,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="14.45" customHeight="1">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="19"/>
     </row>
     <row r="2" spans="1:14" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -7665,7 +7673,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2B31E7-254D-48AD-B04E-DE0E04DB3E4D}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" zoomScale="117" workbookViewId="0">
+    <sheetView zoomScale="117" workbookViewId="0">
       <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
@@ -7704,28 +7712,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="20.45">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="20" t="s">
         <v>218</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="20"/>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="20"/>
-      <c r="T1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+      <c r="T1" s="22"/>
     </row>
     <row r="2" spans="1:32" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -8155,28 +8163,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="16"/>
+      <c r="P1" s="16"/>
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="16"/>
+      <c r="T1" s="16"/>
     </row>
     <row r="2" spans="1:20" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -8392,18 +8400,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
@@ -8481,7 +8489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4E2E4EC-E767-4843-A6BD-026E33879243}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" zoomScale="142" workbookViewId="0">
+    <sheetView zoomScale="142" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -8499,18 +8507,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>294</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">

</xml_diff>

<commit_message>
employee insertion bug resolved
</commit_message>
<xml_diff>
--- a/kiba_labs_data_sheet_new.xlsx
+++ b/kiba_labs_data_sheet_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28706"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28712"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nabeel\AIDIPH-LIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="93" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{25D4CBEA-6389-40A4-9301-35B7527CCDEE}"/>
+  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6E5A380-9CC2-4F9D-8C80-A52C7D1BDCCB}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="17" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organisation_details" sheetId="1" r:id="rId1"/>
@@ -2107,7 +2107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="476">
   <si>
     <t>ORGANISATIONS ESTABLISHMENT AND FINANCIAL DETAILS</t>
   </si>
@@ -2373,16 +2373,25 @@
     <t>Asia/Kolkata</t>
   </si>
   <si>
-    <t>pat02</t>
+    <t>kar</t>
+  </si>
+  <si>
+    <t>karnataka</t>
+  </si>
+  <si>
+    <t>Bangalore</t>
+  </si>
+  <si>
+    <t>ban01</t>
   </si>
   <si>
     <t>No</t>
   </si>
   <si>
-    <t>Boaring road</t>
-  </si>
-  <si>
-    <t>Near Sai Mandir Spti building</t>
+    <t>whitefield</t>
+  </si>
+  <si>
+    <t>1st floor, near btm layout</t>
   </si>
   <si>
     <t>nabeelhassan17808@gmail.com</t>
@@ -2433,24 +2442,24 @@
     <t>Software Development</t>
   </si>
   <si>
+    <t>CC104</t>
+  </si>
+  <si>
+    <t>Application Development</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
     <t>it01</t>
   </si>
   <si>
+    <t>Handles software, hardware, and security systems</t>
+  </si>
+  <si>
     <t>IT002</t>
   </si>
   <si>
-    <t>CC104</t>
-  </si>
-  <si>
-    <t>Application Development</t>
-  </si>
-  <si>
-    <t>IT</t>
-  </si>
-  <si>
-    <t>Handles software, hardware, and security systems</t>
-  </si>
-  <si>
     <t>Information Technology</t>
   </si>
   <si>
@@ -2592,7 +2601,7 @@
     <t>consultant</t>
   </si>
   <si>
-    <t>PT01</t>
+    <t>CN01</t>
   </si>
   <si>
     <t>Part-time employment</t>
@@ -4076,7 +4085,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="G1" workbookViewId="0">
       <selection activeCell="T5" sqref="T5"/>
     </sheetView>
   </sheetViews>
@@ -4363,7 +4372,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>299</v>
+        <v>302</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4379,54 +4388,54 @@
     </row>
     <row r="2" spans="1:12" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>301</v>
+        <v>304</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>302</v>
+        <v>305</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>303</v>
+        <v>306</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>305</v>
+        <v>308</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>306</v>
+        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:12">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E3" s="9">
         <v>45292</v>
@@ -4446,16 +4455,16 @@
     </row>
     <row r="4" spans="1:12">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D4" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E4" s="9">
         <v>45388</v>
@@ -4475,16 +4484,16 @@
     </row>
     <row r="5" spans="1:12">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="D5" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E5" s="9">
         <v>45690</v>
@@ -4533,7 +4542,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4545,7 +4554,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4554,27 +4563,27 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>309</v>
+        <v>312</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>313</v>
+        <v>316</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>314</v>
+        <v>317</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4638,7 +4647,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>307</v>
+        <v>310</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4651,7 +4660,7 @@
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>308</v>
+        <v>311</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4660,54 +4669,54 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>315</v>
+        <v>318</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>316</v>
+        <v>319</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>319</v>
+        <v>322</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>320</v>
+        <v>323</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>321</v>
+        <v>324</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>322</v>
+        <v>325</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>324</v>
+        <v>327</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>325</v>
+        <v>328</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.9">
       <c r="A3" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4740,25 +4749,25 @@
         <v>4000000</v>
       </c>
       <c r="L3" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="O3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="P3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="Q3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
     </row>
   </sheetData>
@@ -4798,7 +4807,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>333</v>
+        <v>336</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4817,7 +4826,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>334</v>
+        <v>337</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4826,45 +4835,45 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>337</v>
+        <v>340</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>338</v>
+        <v>341</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>339</v>
+        <v>342</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>343</v>
+        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>344</v>
+        <v>347</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4873,33 +4882,33 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="E3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="F3" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="J3" s="9">
         <v>45292</v>
       </c>
       <c r="L3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="M3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="O3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="O11" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -4943,7 +4952,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4965,10 +4974,10 @@
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -4977,54 +4986,54 @@
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>349</v>
+        <v>352</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>350</v>
+        <v>353</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>351</v>
+        <v>354</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>352</v>
+        <v>355</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>353</v>
+        <v>356</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>354</v>
+        <v>357</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>355</v>
+        <v>358</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.9">
       <c r="A3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5033,42 +5042,42 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>357</v>
+        <v>360</v>
       </c>
       <c r="F3" t="s">
-        <v>358</v>
+        <v>361</v>
       </c>
       <c r="G3" t="s">
-        <v>359</v>
+        <v>362</v>
       </c>
       <c r="H3" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="K3" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
       <c r="L3" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="M3" s="6" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="O3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="P3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="Q3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="R3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26" spans="13:13">
       <c r="M26" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -5113,7 +5122,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5139,10 +5148,10 @@
     </row>
     <row r="2" spans="1:22" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>365</v>
+        <v>368</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -5151,66 +5160,66 @@
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>366</v>
+        <v>369</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>367</v>
+        <v>370</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>368</v>
+        <v>371</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>369</v>
+        <v>372</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>370</v>
+        <v>373</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>371</v>
+        <v>374</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5219,19 +5228,19 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="F3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="G3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="I3" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -5261,16 +5270,16 @@
         <v>15</v>
       </c>
       <c r="S3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="T3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="U3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="V3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5285,7 +5294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78C55244-73ED-4C00-9AAA-1CE3088AB3F0}">
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView topLeftCell="E8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
@@ -5310,7 +5319,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5328,87 +5337,87 @@
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>379</v>
+        <v>382</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>381</v>
+        <v>384</v>
       </c>
       <c r="E3" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="G3" s="9">
         <v>45292</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="L3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="M3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="O3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -5444,7 +5453,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5457,57 +5466,57 @@
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="1" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>380</v>
+        <v>383</v>
       </c>
       <c r="B3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="C3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="F3" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="G3" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="I3" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -5557,7 +5566,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="14.45" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5579,13 +5588,13 @@
     </row>
     <row r="2" spans="1:24" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>3</v>
@@ -5594,72 +5603,72 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>401</v>
+        <v>404</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>402</v>
+        <v>405</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>403</v>
+        <v>406</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>404</v>
+        <v>407</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>405</v>
+        <v>408</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>406</v>
+        <v>409</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>323</v>
+        <v>326</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>407</v>
+        <v>410</v>
       </c>
       <c r="B3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="C3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -5668,7 +5677,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="G3">
         <v>12</v>
@@ -5704,21 +5713,21 @@
         <v>1</v>
       </c>
       <c r="U3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="V3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="W3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="X3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="6" spans="1:24">
       <c r="D6" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -5757,7 +5766,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>408</v>
+        <v>411</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5770,7 +5779,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>409</v>
+        <v>412</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -5779,31 +5788,31 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>317</v>
+        <v>320</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>318</v>
+        <v>321</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>410</v>
+        <v>413</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>411</v>
+        <v>414</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>412</v>
+        <v>415</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>413</v>
+        <v>416</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>414</v>
+        <v>417</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>415</v>
+        <v>418</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>62</v>
@@ -5826,16 +5835,16 @@
         <v>45657</v>
       </c>
       <c r="F3" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="G3" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
       <c r="H3" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="I3" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="J3" s="9">
         <v>45292</v>
@@ -5864,16 +5873,16 @@
         <v>45657</v>
       </c>
       <c r="F4" t="s">
+        <v>423</v>
+      </c>
+      <c r="G4" t="s">
         <v>420</v>
       </c>
-      <c r="G4" t="s">
-        <v>417</v>
-      </c>
       <c r="H4" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="I4" t="s">
-        <v>421</v>
+        <v>424</v>
       </c>
       <c r="J4" s="9">
         <v>45519</v>
@@ -5902,16 +5911,16 @@
         <v>45657</v>
       </c>
       <c r="F5" t="s">
-        <v>422</v>
+        <v>425</v>
       </c>
       <c r="G5" t="s">
-        <v>423</v>
+        <v>426</v>
       </c>
       <c r="H5" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="I5" t="s">
-        <v>425</v>
+        <v>428</v>
       </c>
       <c r="J5" s="9">
         <v>45426</v>
@@ -5920,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>426</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -5938,7 +5947,7 @@
   <dimension ref="A1:V4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="S11" sqref="S11"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -5959,7 +5968,7 @@
     <col min="14" max="14" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="26.140625" customWidth="1"/>
-    <col min="17" max="17" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="7.42578125" customWidth="1"/>
@@ -6139,40 +6148,40 @@
         <v>37</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="H4" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="I4" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="J4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="L4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="M4" t="s">
         <v>83</v>
       </c>
       <c r="N4" t="s">
+        <v>93</v>
+      </c>
+      <c r="O4" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q4" t="s">
         <v>90</v>
       </c>
-      <c r="O4" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>81</v>
-      </c>
       <c r="R4">
-        <v>800002</v>
+        <v>240568</v>
       </c>
       <c r="S4" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="V4" t="s">
         <v>87</v>
@@ -6238,7 +6247,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.45" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6261,10 +6270,10 @@
     </row>
     <row r="2" spans="1:34" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>335</v>
+        <v>338</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>336</v>
+        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -6273,102 +6282,102 @@
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>428</v>
+        <v>431</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>429</v>
+        <v>432</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="Q2" s="12" t="s">
-        <v>440</v>
+        <v>443</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>441</v>
+        <v>444</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>442</v>
+        <v>445</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>443</v>
+        <v>446</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>445</v>
+        <v>448</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>446</v>
+        <v>449</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>447</v>
+        <v>450</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>448</v>
+        <v>451</v>
       </c>
       <c r="Z2" s="12" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="AA2" s="12" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="AC2" s="12" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="AD2" s="12" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:34">
       <c r="A3" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -6377,7 +6386,7 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -6386,13 +6395,13 @@
         <v>500</v>
       </c>
       <c r="H3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="I3" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="J3" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="L3">
         <v>15</v>
@@ -6416,10 +6425,10 @@
         <v>30</v>
       </c>
       <c r="U3" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="W3" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="X3" t="b">
         <v>0</v>
@@ -6440,16 +6449,16 @@
         <v>2</v>
       </c>
       <c r="AE3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AF3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AG3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AH3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6491,7 +6500,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6514,10 +6523,10 @@
     </row>
     <row r="2" spans="1:19" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -6526,48 +6535,48 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>436</v>
+        <v>439</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>437</v>
+        <v>440</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15">
       <c r="A3" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="B3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -6576,10 +6585,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -6594,27 +6603,27 @@
         <v>8.5</v>
       </c>
       <c r="L3" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="M3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="O3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="P3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="15">
       <c r="A4" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="B4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -6623,10 +6632,10 @@
         <v>37</v>
       </c>
       <c r="E4" s="15" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -6644,19 +6653,19 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="M4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="N4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="O4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="P4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6692,7 +6701,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>427</v>
+        <v>430</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6705,121 +6714,121 @@
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>340</v>
+        <v>343</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>341</v>
+        <v>344</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>342</v>
+        <v>345</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>356</v>
+        <v>359</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E3" s="9">
         <v>45747</v>
       </c>
       <c r="G3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B4" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="D4" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="E4" s="9">
         <v>45717</v>
       </c>
       <c r="G4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="D5" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E5" s="9">
         <v>45721</v>
       </c>
       <c r="G5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="H5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="I5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="J5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
     </row>
   </sheetData>
@@ -6834,8 +6843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0F9FA7-C132-473D-AA3C-1F3E68753829}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -6854,7 +6863,7 @@
   <sheetData>
     <row r="1" spans="1:11" ht="21" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -6869,13 +6878,13 @@
     </row>
     <row r="2" spans="1:11">
       <c r="A2" s="14" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D2" s="14" t="s">
         <v>3</v>
@@ -6884,33 +6893,33 @@
         <v>7</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" ht="28.9">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="30.75">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>34</v>
@@ -6919,33 +6928,29 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="G3" t="s">
-        <v>107</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>109</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
       <c r="J3" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="K3" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="28.9">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B4" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>34</v>
@@ -6954,16 +6959,16 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="G4" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J4" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="K4" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -6979,8 +6984,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33BD60CA-9150-40C0-B868-C9DA9FAE1363}">
   <dimension ref="A1:AH5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" customHeight="1"/>
@@ -7021,7 +7026,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="21" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -7049,13 +7054,13 @@
     </row>
     <row r="2" spans="1:34" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>3</v>
@@ -7064,102 +7069,102 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="P2" s="12" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="S2" s="12" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="T2" s="12" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="U2" s="12" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="V2" s="12" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="X2" s="12" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="AB2" s="12" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="AH2" s="12" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:34" ht="28.9">
       <c r="A3" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B3" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="C3" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -7168,25 +7173,25 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="G3" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="I3">
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="K3" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L3" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M3" t="s">
         <v>82</v>
@@ -7195,25 +7200,25 @@
         <v>81</v>
       </c>
       <c r="O3" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="P3" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="R3" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="S3" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="T3" s="9">
         <v>36951</v>
       </c>
       <c r="U3" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="V3" s="4" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="W3" s="4" t="s">
         <v>86</v>
@@ -7222,10 +7227,10 @@
         <v>9852369870</v>
       </c>
       <c r="Y3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="Z3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="AA3">
         <v>9608020606</v>
@@ -7245,13 +7250,13 @@
     </row>
     <row r="4" spans="1:34" ht="14.45">
       <c r="A4" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="C4" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
@@ -7260,25 +7265,25 @@
         <v>37</v>
       </c>
       <c r="F4" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G4" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="J4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="K4" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="L4" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="M4" t="s">
         <v>82</v>
@@ -7287,37 +7292,37 @@
         <v>81</v>
       </c>
       <c r="O4" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="P4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="R4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="S4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="T4" s="9">
         <v>35553</v>
       </c>
       <c r="U4" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="V4" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="W4" s="4" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="X4">
         <v>9899559598</v>
       </c>
       <c r="Y4" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="Z4" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AA4">
         <v>9899559598</v>
@@ -7332,10 +7337,10 @@
         <v>45691</v>
       </c>
       <c r="AF4" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AG4" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AH4">
         <v>60</v>
@@ -7343,13 +7348,13 @@
     </row>
     <row r="5" spans="1:34">
       <c r="A5" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="B5" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="C5" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D5" t="s">
         <v>34</v>
@@ -7358,64 +7363,64 @@
         <v>37</v>
       </c>
       <c r="F5" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="G5" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="H5" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="I5">
         <v>7</v>
       </c>
       <c r="J5" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="K5" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="L5" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="M5" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="N5" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="O5" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="P5" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="R5" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="S5" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="T5" s="9">
         <v>33299</v>
       </c>
       <c r="U5" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="V5" s="4" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="W5" s="4" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="X5">
         <v>9608020606</v>
       </c>
       <c r="Y5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="Z5" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="AA5">
         <v>9852369870</v>
@@ -7430,10 +7435,10 @@
         <v>44961</v>
       </c>
       <c r="AF5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="AG5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="AH5">
         <v>60</v>
@@ -7484,7 +7489,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="14.45" customHeight="1">
       <c r="A1" s="17" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="B1" s="18"/>
       <c r="C1" s="18"/>
@@ -7502,163 +7507,163 @@
     </row>
     <row r="2" spans="1:14" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I2" s="12" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D3" s="9">
         <v>45649</v>
       </c>
       <c r="E3" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F3" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G3" t="b">
         <v>0</v>
       </c>
       <c r="I3" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="J3" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="L3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M3">
         <v>8964</v>
       </c>
       <c r="N3" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D4" s="9">
         <v>44177</v>
       </c>
       <c r="E4" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F4" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G4" t="b">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="I4" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="J4" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="L4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="M4">
         <v>3245</v>
       </c>
       <c r="N4" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
     </row>
     <row r="5" spans="1:14">
       <c r="A5" s="7" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D5" s="9">
         <v>45177</v>
       </c>
       <c r="E5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F5" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G5" t="b">
         <v>0</v>
       </c>
       <c r="I5" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="J5" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="L5" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="M5">
         <v>4435</v>
       </c>
       <c r="N5" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
     </row>
   </sheetData>
@@ -7713,7 +7718,7 @@
   <sheetData>
     <row r="1" spans="1:32" ht="20.45">
       <c r="A1" s="20" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="B1" s="21"/>
       <c r="C1" s="21"/>
@@ -7737,16 +7742,16 @@
     </row>
     <row r="2" spans="1:32" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>21</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>8</v>
@@ -7776,78 +7781,78 @@
         <v>16</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>23</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="V2" s="1" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="W2" s="1" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="X2" s="1" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="Y2" s="1" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="Z2" s="1" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="AD2" s="1" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="28.9">
       <c r="A3" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="B3" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="C3" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E3" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -7856,37 +7861,37 @@
         <v>32554</v>
       </c>
       <c r="H3" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I3">
         <v>368821018</v>
       </c>
       <c r="J3" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K3" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="L3" t="s">
         <v>43</v>
       </c>
       <c r="M3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="N3" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>244</v>
+        <v>247</v>
       </c>
       <c r="Q3" s="9">
         <v>43997</v>
       </c>
       <c r="R3" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="T3" t="b">
         <v>0</v>
@@ -7907,42 +7912,42 @@
         <v>36221</v>
       </c>
       <c r="Z3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="AA3" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AB3" t="b">
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="AD3" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="AE3" s="9">
         <v>36221</v>
       </c>
       <c r="AF3" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="28.9">
       <c r="A4" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="B4" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
@@ -7951,37 +7956,37 @@
         <v>32554</v>
       </c>
       <c r="H4" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I4">
         <v>758833459</v>
       </c>
       <c r="J4" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K4" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="L4" t="s">
         <v>43</v>
       </c>
       <c r="M4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="N4" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="Q4" s="9">
         <v>44389</v>
       </c>
       <c r="R4" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="T4" t="b">
         <v>0</v>
@@ -7999,42 +8004,42 @@
         <v>37440</v>
       </c>
       <c r="Z4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AA4" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AB4" t="b">
         <v>1</v>
       </c>
       <c r="AC4" t="s">
-        <v>248</v>
+        <v>251</v>
       </c>
       <c r="AD4" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="AE4" s="9">
         <v>36195</v>
       </c>
       <c r="AF4" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:32" ht="28.9">
       <c r="A5" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B5" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -8043,37 +8048,37 @@
         <v>32554</v>
       </c>
       <c r="H5" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="I5">
         <v>223478905</v>
       </c>
       <c r="J5" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="K5" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="L5" t="s">
         <v>43</v>
       </c>
       <c r="M5" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="N5" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>249</v>
+        <v>252</v>
       </c>
       <c r="Q5" s="9">
         <v>45566</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>245</v>
+        <v>248</v>
       </c>
       <c r="T5" t="b">
         <v>0</v>
@@ -8091,25 +8096,25 @@
         <v>33451</v>
       </c>
       <c r="Z5" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AA5" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="AB5" t="b">
         <v>1</v>
       </c>
       <c r="AC5" t="s">
-        <v>250</v>
+        <v>253</v>
       </c>
       <c r="AD5" s="7" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="AE5" s="9">
         <v>37289</v>
       </c>
       <c r="AF5" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
     </row>
   </sheetData>
@@ -8126,7 +8131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B01DC832-5353-409E-939C-876616421212}">
   <dimension ref="A1:T8"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="137" workbookViewId="0">
+    <sheetView zoomScale="137" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
@@ -8164,7 +8169,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8188,7 +8193,7 @@
     </row>
     <row r="2" spans="1:20" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -8197,60 +8202,60 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>256</v>
+        <v>259</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>257</v>
+        <v>260</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="J2" s="12" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="K2" s="12" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="L2" s="12" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="M2" s="12" t="s">
-        <v>263</v>
+        <v>266</v>
       </c>
       <c r="N2" s="12" t="s">
-        <v>264</v>
+        <v>267</v>
       </c>
       <c r="O2" s="12" t="s">
-        <v>265</v>
+        <v>268</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="R2" s="12" t="s">
-        <v>268</v>
+        <v>271</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>269</v>
+        <v>272</v>
       </c>
       <c r="T2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>270</v>
+        <v>273</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -8259,19 +8264,19 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="E3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F3" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G3" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="J3" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -8289,24 +8294,24 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="Q3" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
-        <v>277</v>
+        <v>280</v>
       </c>
       <c r="T3" t="s">
-        <v>278</v>
+        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>279</v>
+        <v>282</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -8315,22 +8320,22 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="E4" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="F4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G4" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="I4" t="s">
-        <v>281</v>
+        <v>284</v>
       </c>
       <c r="J4" t="s">
-        <v>275</v>
+        <v>278</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -8348,24 +8353,24 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="Q4" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>280</v>
+        <v>283</v>
       </c>
       <c r="T4" t="s">
-        <v>282</v>
+        <v>285</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="E8" t="s">
-        <v>283</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -8401,7 +8406,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8415,7 +8420,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -8424,30 +8429,30 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>286</v>
+        <v>289</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>287</v>
+        <v>290</v>
       </c>
       <c r="H2" s="12" t="s">
-        <v>288</v>
+        <v>291</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>289</v>
+        <v>292</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -8456,10 +8461,10 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="E3" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="F3">
         <v>300000</v>
@@ -8471,7 +8476,7 @@
         <v>45292</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>276</v>
+        <v>279</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -8508,7 +8513,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>294</v>
+        <v>297</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8522,48 +8527,48 @@
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>284</v>
+        <v>287</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>285</v>
+        <v>288</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>255</v>
+        <v>258</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>295</v>
+        <v>298</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>296</v>
+        <v>299</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>297</v>
+        <v>300</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>266</v>
+        <v>269</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>298</v>
+        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>291</v>
+        <v>294</v>
       </c>
       <c r="B3" t="s">
-        <v>292</v>
+        <v>295</v>
       </c>
       <c r="C3" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="D3" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>

<commit_message>
resolved data injestion bugs
</commit_message>
<xml_diff>
--- a/kiba_labs_data_sheet_new.xlsx
+++ b/kiba_labs_data_sheet_new.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28712"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28715"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Nabeel\AIDIPH-LIVE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="111" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D6E5A380-9CC2-4F9D-8C80-A52C7D1BDCCB}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="13_ncr:1_{A5A4070F-D38F-4014-BE47-610EF6C61807}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D71ADF63-0E4D-486B-9F29-EA0B102EB16A}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="organisation_details" sheetId="1" r:id="rId1"/>
@@ -2107,7 +2107,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="476">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="862" uniqueCount="475">
   <si>
     <t>ORGANISATIONS ESTABLISHMENT AND FINANCIAL DETAILS</t>
   </si>
@@ -2830,9 +2830,6 @@
   </si>
   <si>
     <t>parent_name_in_pan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> IT2024BR</t>
   </si>
   <si>
     <t>employee_bank</t>
@@ -3760,7 +3757,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -3801,6 +3798,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4085,8 +4085,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AE8"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T5" sqref="T5"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -4372,7 +4372,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4391,37 +4391,37 @@
         <v>125</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>303</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>287</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>304</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>305</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="1" t="s">
         <v>308</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -4432,10 +4432,10 @@
         <v>184</v>
       </c>
       <c r="C3" t="s">
+        <v>293</v>
+      </c>
+      <c r="D3" t="s">
         <v>294</v>
-      </c>
-      <c r="D3" t="s">
-        <v>295</v>
       </c>
       <c r="E3" s="9">
         <v>45292</v>
@@ -4461,10 +4461,10 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D4" t="s">
         <v>294</v>
-      </c>
-      <c r="D4" t="s">
-        <v>295</v>
       </c>
       <c r="E4" s="9">
         <v>45388</v>
@@ -4490,10 +4490,10 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
+        <v>293</v>
+      </c>
+      <c r="D5" t="s">
         <v>294</v>
-      </c>
-      <c r="D5" t="s">
-        <v>295</v>
       </c>
       <c r="E5" s="9">
         <v>45690</v>
@@ -4542,7 +4542,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4554,7 +4554,7 @@
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4563,27 +4563,27 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>311</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>312</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>314</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>315</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>316</v>
-      </c>
       <c r="I2" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4647,7 +4647,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4660,7 +4660,7 @@
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4669,54 +4669,54 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>317</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>318</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>319</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>321</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>322</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>323</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>324</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="1" t="s">
         <v>325</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="1" t="s">
         <v>326</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>328</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>329</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="1" t="s">
         <v>331</v>
-      </c>
-      <c r="R2" s="1" t="s">
-        <v>332</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.9">
       <c r="A3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4749,7 +4749,7 @@
         <v>4000000</v>
       </c>
       <c r="L3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="M3" t="b">
         <v>1</v>
@@ -4767,7 +4767,7 @@
         <v>156</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
   </sheetData>
@@ -4807,7 +4807,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4826,7 +4826,7 @@
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -4835,45 +4835,45 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="1" t="s">
         <v>339</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="12" t="s">
         <v>340</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>341</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="J2" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="L2" s="12" t="s">
         <v>342</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="J2" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>343</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>344</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>345</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>346</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -4882,13 +4882,13 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E3" t="s">
         <v>348</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>349</v>
-      </c>
-      <c r="F3" t="s">
-        <v>350</v>
       </c>
       <c r="J3" s="9">
         <v>45292</v>
@@ -4908,7 +4908,7 @@
     </row>
     <row r="11" spans="1:15">
       <c r="O11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -4952,7 +4952,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -4974,10 +4974,10 @@
     </row>
     <row r="2" spans="1:18" ht="15.6">
       <c r="A2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -4986,54 +4986,54 @@
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>352</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>353</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>354</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="12" t="s">
         <v>355</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>356</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="1" t="s">
         <v>357</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>358</v>
-      </c>
       <c r="L2" s="1" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="O2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="P2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="R2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="28.9">
       <c r="A3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" t="s">
         <v>348</v>
-      </c>
-      <c r="B3" t="s">
-        <v>349</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -5042,25 +5042,25 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
+        <v>359</v>
+      </c>
+      <c r="F3" t="s">
         <v>360</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>361</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>362</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>363</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>364</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" s="6" t="s">
         <v>365</v>
-      </c>
-      <c r="M3" s="6" t="s">
-        <v>366</v>
       </c>
       <c r="O3" t="s">
         <v>154</v>
@@ -5077,7 +5077,7 @@
     </row>
     <row r="26" spans="13:13">
       <c r="M26" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -5122,7 +5122,7 @@
   <sheetData>
     <row r="1" spans="1:22" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5148,10 +5148,10 @@
     </row>
     <row r="2" spans="1:22" ht="15.6">
       <c r="A2" s="12" t="s">
+        <v>366</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>367</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>368</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -5172,46 +5172,46 @@
         <v>191</v>
       </c>
       <c r="I2" s="12" t="s">
+        <v>368</v>
+      </c>
+      <c r="J2" s="12" t="s">
         <v>369</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>370</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>374</v>
-      </c>
-      <c r="O2" s="12" t="s">
-        <v>375</v>
       </c>
       <c r="P2" s="12" t="s">
         <v>148</v>
       </c>
       <c r="Q2" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>377</v>
-      </c>
       <c r="S2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="U2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="V2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:22">
@@ -5240,7 +5240,7 @@
         <v>184</v>
       </c>
       <c r="I3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -5319,7 +5319,7 @@
   <sheetData>
     <row r="1" spans="1:15" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5337,66 +5337,66 @@
     </row>
     <row r="2" spans="1:15" ht="15.6">
       <c r="A2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>339</v>
-      </c>
       <c r="C2" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
+        <v>325</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>291</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>292</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>382</v>
-      </c>
       <c r="J2" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>330</v>
       </c>
-      <c r="K2" s="1" t="s">
-        <v>331</v>
-      </c>
       <c r="L2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:15">
       <c r="A3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" t="s">
         <v>348</v>
       </c>
-      <c r="B3" t="s">
-        <v>349</v>
-      </c>
       <c r="C3" t="s">
+        <v>382</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>383</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" t="s">
         <v>384</v>
-      </c>
-      <c r="E3" t="s">
-        <v>385</v>
       </c>
       <c r="G3" s="9">
         <v>45292</v>
@@ -5453,7 +5453,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5466,36 +5466,36 @@
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="1" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>125</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>385</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="1" t="s">
         <v>387</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>388</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>389</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="3" spans="1:9">
       <c r="A3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B3" t="s">
         <v>154</v>
@@ -5504,19 +5504,19 @@
         <v>156</v>
       </c>
       <c r="D3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F3" t="s">
+        <v>390</v>
+      </c>
+      <c r="G3" t="s">
         <v>391</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="I3" t="s">
         <v>393</v>
-      </c>
-      <c r="I3" t="s">
-        <v>394</v>
       </c>
     </row>
   </sheetData>
@@ -5566,7 +5566,7 @@
   <sheetData>
     <row r="1" spans="1:24" ht="14.45" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5588,13 +5588,13 @@
     </row>
     <row r="2" spans="1:24" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="D2" s="12" t="s">
         <v>3</v>
@@ -5603,72 +5603,72 @@
         <v>7</v>
       </c>
       <c r="F2" s="12" t="s">
+        <v>395</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="1" t="s">
         <v>397</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>398</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="1" t="s">
         <v>403</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="12" t="s">
         <v>404</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="1" t="s">
         <v>406</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="S2" s="12" t="s">
-        <v>409</v>
-      </c>
       <c r="T2" s="1" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="U2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="V2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="W2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="X2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:24">
       <c r="A3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C3" t="s">
         <v>348</v>
-      </c>
-      <c r="C3" t="s">
-        <v>349</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
@@ -5677,7 +5677,7 @@
         <v>37</v>
       </c>
       <c r="F3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="G3">
         <v>12</v>
@@ -5727,7 +5727,7 @@
     </row>
     <row r="6" spans="1:24">
       <c r="D6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -5766,7 +5766,7 @@
   <sheetData>
     <row r="1" spans="1:13" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -5779,7 +5779,7 @@
     </row>
     <row r="2" spans="1:13" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -5788,31 +5788,31 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>319</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="E2" s="12" t="s">
-        <v>321</v>
-      </c>
       <c r="F2" s="12" t="s">
+        <v>412</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>413</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="12" t="s">
         <v>414</v>
-      </c>
-      <c r="H2" s="12" t="s">
-        <v>415</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="J2" s="12" t="s">
+        <v>415</v>
+      </c>
+      <c r="K2" s="12" t="s">
         <v>416</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="1" t="s">
         <v>417</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>418</v>
       </c>
       <c r="M2" s="1" t="s">
         <v>62</v>
@@ -5835,16 +5835,16 @@
         <v>45657</v>
       </c>
       <c r="F3" t="s">
+        <v>418</v>
+      </c>
+      <c r="G3" t="s">
         <v>419</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>420</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>421</v>
-      </c>
-      <c r="I3" t="s">
-        <v>422</v>
       </c>
       <c r="J3" s="9">
         <v>45292</v>
@@ -5873,16 +5873,16 @@
         <v>45657</v>
       </c>
       <c r="F4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G4" t="s">
+        <v>419</v>
+      </c>
+      <c r="H4" t="s">
+        <v>420</v>
+      </c>
+      <c r="I4" t="s">
         <v>423</v>
-      </c>
-      <c r="G4" t="s">
-        <v>420</v>
-      </c>
-      <c r="H4" t="s">
-        <v>421</v>
-      </c>
-      <c r="I4" t="s">
-        <v>424</v>
       </c>
       <c r="J4" s="9">
         <v>45519</v>
@@ -5911,16 +5911,16 @@
         <v>45657</v>
       </c>
       <c r="F5" t="s">
+        <v>424</v>
+      </c>
+      <c r="G5" t="s">
         <v>425</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>426</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>427</v>
-      </c>
-      <c r="I5" t="s">
-        <v>428</v>
       </c>
       <c r="J5" s="9">
         <v>45426</v>
@@ -5929,7 +5929,7 @@
         <v>0</v>
       </c>
       <c r="M5" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -6247,7 +6247,7 @@
   <sheetData>
     <row r="1" spans="1:34" ht="14.45" customHeight="1">
       <c r="A1" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6270,10 +6270,10 @@
     </row>
     <row r="2" spans="1:34" ht="15.6">
       <c r="A2" s="12" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>338</v>
-      </c>
-      <c r="B2" s="12" t="s">
-        <v>339</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -6282,102 +6282,102 @@
         <v>7</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>430</v>
+      </c>
+      <c r="F2" s="12" t="s">
         <v>431</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="1" t="s">
         <v>432</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="12" t="s">
         <v>433</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="1" t="s">
         <v>434</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>435</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>436</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>439</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="12" t="s">
         <v>440</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="12" t="s">
         <v>441</v>
       </c>
-      <c r="P2" s="12" t="s">
+      <c r="Q2" s="12" t="s">
         <v>442</v>
       </c>
-      <c r="Q2" s="12" t="s">
+      <c r="R2" s="1" t="s">
         <v>443</v>
       </c>
-      <c r="R2" s="1" t="s">
+      <c r="S2" s="1" t="s">
         <v>444</v>
       </c>
-      <c r="S2" s="1" t="s">
+      <c r="T2" s="1" t="s">
         <v>445</v>
       </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>446</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>447</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>448</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="12" t="s">
         <v>449</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="Y2" s="1" t="s">
         <v>450</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="12" t="s">
         <v>451</v>
       </c>
-      <c r="Z2" s="12" t="s">
+      <c r="AA2" s="12" t="s">
         <v>452</v>
       </c>
-      <c r="AA2" s="12" t="s">
+      <c r="AB2" s="12" t="s">
         <v>453</v>
       </c>
-      <c r="AB2" s="12" t="s">
+      <c r="AC2" s="12" t="s">
         <v>454</v>
       </c>
-      <c r="AC2" s="12" t="s">
+      <c r="AD2" s="12" t="s">
         <v>455</v>
       </c>
-      <c r="AD2" s="12" t="s">
-        <v>456</v>
-      </c>
       <c r="AE2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="AF2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="AF2" s="1" t="s">
+      <c r="AG2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="AG2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="AH2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:34">
       <c r="A3" t="s">
+        <v>347</v>
+      </c>
+      <c r="B3" t="s">
         <v>348</v>
-      </c>
-      <c r="B3" t="s">
-        <v>349</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -6386,7 +6386,7 @@
         <v>37</v>
       </c>
       <c r="E3" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="F3" t="b">
         <v>1</v>
@@ -6395,13 +6395,13 @@
         <v>500</v>
       </c>
       <c r="H3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="I3" t="s">
+        <v>457</v>
+      </c>
+      <c r="J3" t="s">
         <v>458</v>
-      </c>
-      <c r="J3" t="s">
-        <v>459</v>
       </c>
       <c r="L3">
         <v>15</v>
@@ -6425,10 +6425,10 @@
         <v>30</v>
       </c>
       <c r="U3" t="s">
+        <v>459</v>
+      </c>
+      <c r="W3" t="s">
         <v>460</v>
-      </c>
-      <c r="W3" t="s">
-        <v>461</v>
       </c>
       <c r="X3" t="b">
         <v>0</v>
@@ -6500,7 +6500,7 @@
   <sheetData>
     <row r="1" spans="1:19" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6523,10 +6523,10 @@
     </row>
     <row r="2" spans="1:19" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>3</v>
@@ -6535,48 +6535,48 @@
         <v>7</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>463</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="H2" s="12" t="s">
         <v>464</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="I2" s="12" t="s">
         <v>437</v>
       </c>
-      <c r="H2" s="12" t="s">
-        <v>465</v>
-      </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="1" t="s">
         <v>438</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="1" t="s">
         <v>439</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>440</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="P2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:19" ht="15">
       <c r="A3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="C3" t="s">
         <v>34</v>
@@ -6585,10 +6585,10 @@
         <v>37</v>
       </c>
       <c r="E3" s="15" t="s">
+        <v>466</v>
+      </c>
+      <c r="F3" s="15" t="s">
         <v>467</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>468</v>
       </c>
       <c r="H3">
         <v>60</v>
@@ -6603,7 +6603,7 @@
         <v>8.5</v>
       </c>
       <c r="L3" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="M3" t="s">
         <v>154</v>
@@ -6620,10 +6620,10 @@
     </row>
     <row r="4" spans="1:19" ht="15">
       <c r="A4" t="s">
+        <v>469</v>
+      </c>
+      <c r="B4" t="s">
         <v>470</v>
-      </c>
-      <c r="B4" t="s">
-        <v>471</v>
       </c>
       <c r="C4" t="s">
         <v>34</v>
@@ -6632,10 +6632,10 @@
         <v>37</v>
       </c>
       <c r="E4" s="15" t="s">
+        <v>471</v>
+      </c>
+      <c r="F4" s="15" t="s">
         <v>472</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>473</v>
       </c>
       <c r="G4">
         <v>2</v>
@@ -6653,7 +6653,7 @@
         <v>8</v>
       </c>
       <c r="L4" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="M4" t="s">
         <v>154</v>
@@ -6701,7 +6701,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -6720,28 +6720,28 @@
         <v>191</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E2" s="12" t="s">
+        <v>290</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="G2" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>343</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>344</v>
       </c>
-      <c r="I2" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="J2" s="1" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -6752,10 +6752,10 @@
         <v>170</v>
       </c>
       <c r="C3" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E3" s="9">
         <v>45747</v>
@@ -6781,10 +6781,10 @@
         <v>184</v>
       </c>
       <c r="C4" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D4" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E4" s="9">
         <v>45717</v>
@@ -6810,10 +6810,10 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E5" s="9">
         <v>45721</v>
@@ -6843,7 +6843,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D0F9FA7-C132-473D-AA3C-1F3E68753829}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -7678,8 +7678,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD2B31E7-254D-48AD-B04E-DE0E04DB3E4D}">
   <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="AB9" sqref="AB9"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -7838,7 +7838,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:32" ht="28.9">
+    <row r="3" spans="1:32" ht="30.75">
       <c r="A3" t="s">
         <v>183</v>
       </c>
@@ -7846,13 +7846,13 @@
         <v>184</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>241</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>242</v>
       </c>
       <c r="F3" t="s">
         <v>39</v>
@@ -7861,16 +7861,16 @@
         <v>32554</v>
       </c>
       <c r="H3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I3">
         <v>368821018</v>
       </c>
       <c r="J3" t="s">
+        <v>243</v>
+      </c>
+      <c r="K3" t="s">
         <v>244</v>
-      </c>
-      <c r="K3" t="s">
-        <v>245</v>
       </c>
       <c r="L3" t="s">
         <v>43</v>
@@ -7879,19 +7879,19 @@
         <v>186</v>
       </c>
       <c r="N3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O3" t="b">
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="Q3" s="9">
         <v>43997</v>
       </c>
       <c r="R3" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T3" t="b">
         <v>0</v>
@@ -7921,7 +7921,7 @@
         <v>1</v>
       </c>
       <c r="AC3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="AD3" t="s">
         <v>186</v>
@@ -7933,7 +7933,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="4" spans="1:32" ht="28.9">
+    <row r="4" spans="1:32" ht="30.75">
       <c r="A4" t="s">
         <v>169</v>
       </c>
@@ -7941,13 +7941,13 @@
         <v>170</v>
       </c>
       <c r="C4" t="s">
-        <v>241</v>
+        <v>49</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" t="s">
         <v>39</v>
@@ -7956,16 +7956,16 @@
         <v>32554</v>
       </c>
       <c r="H4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I4">
         <v>758833459</v>
       </c>
       <c r="J4" t="s">
+        <v>243</v>
+      </c>
+      <c r="K4" t="s">
         <v>244</v>
-      </c>
-      <c r="K4" t="s">
-        <v>245</v>
       </c>
       <c r="L4" t="s">
         <v>43</v>
@@ -7974,19 +7974,19 @@
         <v>172</v>
       </c>
       <c r="N4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O4" t="b">
         <v>1</v>
       </c>
       <c r="P4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="Q4" s="9">
         <v>44389</v>
       </c>
       <c r="R4" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T4" t="b">
         <v>0</v>
@@ -8013,7 +8013,7 @@
         <v>1</v>
       </c>
       <c r="AC4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="AD4" t="s">
         <v>172</v>
@@ -8025,7 +8025,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="5" spans="1:32" ht="28.9">
+    <row r="5" spans="1:32" ht="30.75">
       <c r="A5" t="s">
         <v>154</v>
       </c>
@@ -8033,13 +8033,13 @@
         <v>156</v>
       </c>
       <c r="C5" t="s">
-        <v>241</v>
+        <v>49</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>50</v>
       </c>
       <c r="E5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -8048,16 +8048,16 @@
         <v>32554</v>
       </c>
       <c r="H5" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="I5">
         <v>223478905</v>
       </c>
       <c r="J5" t="s">
+        <v>243</v>
+      </c>
+      <c r="K5" t="s">
         <v>244</v>
-      </c>
-      <c r="K5" t="s">
-        <v>245</v>
       </c>
       <c r="L5" t="s">
         <v>43</v>
@@ -8066,19 +8066,19 @@
         <v>158</v>
       </c>
       <c r="N5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="O5" t="b">
         <v>1</v>
       </c>
       <c r="P5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="Q5" s="9">
         <v>45566</v>
       </c>
       <c r="R5" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="T5" t="b">
         <v>0</v>
@@ -8105,7 +8105,7 @@
         <v>1</v>
       </c>
       <c r="AC5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="AD5" s="7" t="s">
         <v>158</v>
@@ -8114,7 +8114,7 @@
         <v>37289</v>
       </c>
       <c r="AF5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
@@ -8169,7 +8169,7 @@
   <sheetData>
     <row r="1" spans="1:20" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8193,7 +8193,7 @@
     </row>
     <row r="2" spans="1:20" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -8202,52 +8202,52 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="F2" s="12" t="s">
         <v>258</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="G2" s="12" t="s">
         <v>259</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="H2" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>261</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="12" t="s">
         <v>262</v>
       </c>
-      <c r="J2" s="12" t="s">
+      <c r="K2" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="K2" s="12" t="s">
+      <c r="L2" s="12" t="s">
         <v>264</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="12" t="s">
         <v>265</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="N2" s="12" t="s">
         <v>266</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>267</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="P2" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>269</v>
       </c>
-      <c r="Q2" s="1" t="s">
+      <c r="R2" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="1" t="s">
         <v>271</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="T2" s="1" t="s">
         <v>99</v>
@@ -8255,7 +8255,7 @@
     </row>
     <row r="3" spans="1:20">
       <c r="A3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -8264,19 +8264,19 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
+        <v>273</v>
+      </c>
+      <c r="E3" t="s">
         <v>274</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>275</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>276</v>
       </c>
-      <c r="G3" t="s">
+      <c r="J3" t="s">
         <v>277</v>
-      </c>
-      <c r="J3" t="s">
-        <v>278</v>
       </c>
       <c r="K3" t="b">
         <v>1</v>
@@ -8294,24 +8294,24 @@
         <v>1</v>
       </c>
       <c r="P3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R3">
         <v>0</v>
       </c>
       <c r="S3" t="s">
+        <v>279</v>
+      </c>
+      <c r="T3" t="s">
         <v>280</v>
-      </c>
-      <c r="T3" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="4" spans="1:20">
       <c r="A4" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
@@ -8320,22 +8320,22 @@
         <v>37</v>
       </c>
       <c r="D4" t="s">
+        <v>282</v>
+      </c>
+      <c r="E4" t="s">
+        <v>274</v>
+      </c>
+      <c r="F4" t="s">
+        <v>275</v>
+      </c>
+      <c r="G4" t="s">
+        <v>276</v>
+      </c>
+      <c r="I4" t="s">
         <v>283</v>
       </c>
-      <c r="E4" t="s">
-        <v>275</v>
-      </c>
-      <c r="F4" t="s">
-        <v>276</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="J4" t="s">
         <v>277</v>
-      </c>
-      <c r="I4" t="s">
-        <v>284</v>
-      </c>
-      <c r="J4" t="s">
-        <v>278</v>
       </c>
       <c r="K4" t="b">
         <v>1</v>
@@ -8353,24 +8353,24 @@
         <v>0</v>
       </c>
       <c r="P4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="Q4" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
       <c r="S4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="T4" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="8" spans="1:20">
       <c r="E8" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -8406,7 +8406,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8420,7 +8420,7 @@
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>3</v>
@@ -8429,30 +8429,30 @@
         <v>7</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>99</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>288</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>289</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="12" t="s">
         <v>290</v>
       </c>
-      <c r="H2" s="12" t="s">
+      <c r="I2" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>292</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>293</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
@@ -8461,10 +8461,10 @@
         <v>37</v>
       </c>
       <c r="D3" t="s">
+        <v>294</v>
+      </c>
+      <c r="E3" t="s">
         <v>295</v>
-      </c>
-      <c r="E3" t="s">
-        <v>296</v>
       </c>
       <c r="F3">
         <v>300000</v>
@@ -8476,7 +8476,7 @@
         <v>45292</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="J3" t="b">
         <v>1</v>
@@ -8513,7 +8513,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="20.45">
       <c r="A1" s="16" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B1" s="16"/>
       <c r="C1" s="16"/>
@@ -8527,48 +8527,48 @@
     </row>
     <row r="2" spans="1:10" ht="15.6">
       <c r="A2" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="B2" s="12" t="s">
         <v>287</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>288</v>
-      </c>
       <c r="C2" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>257</v>
       </c>
-      <c r="D2" s="12" t="s">
-        <v>258</v>
-      </c>
       <c r="E2" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>299</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="H2" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="J2" s="1" t="s">
         <v>300</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>269</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
+        <v>293</v>
+      </c>
+      <c r="B3" t="s">
         <v>294</v>
       </c>
-      <c r="B3" t="s">
-        <v>295</v>
-      </c>
       <c r="C3" t="s">
+        <v>273</v>
+      </c>
+      <c r="D3" t="s">
         <v>274</v>
-      </c>
-      <c r="D3" t="s">
-        <v>275</v>
       </c>
       <c r="E3">
         <v>1</v>

</xml_diff>